<commit_message>
Çoklu revizede ve çoklu kayıtta hata düzeltmeleri, çoklu kayıt fonksiyonunu yeniden async fonksiyon kullanarak yazdım.
</commit_message>
<xml_diff>
--- a/coklurevize.xlsx
+++ b/coklurevize.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Sicil no</t>
   </si>
@@ -21,13 +21,22 @@
     <t xml:space="preserve">Yeni rol</t>
   </si>
   <si>
+    <t>T49</t>
+  </si>
+  <si>
     <t>Bireysel,Yazılımcı,Yardımcı</t>
   </si>
   <si>
-    <t>Bireysel,Araştırmacı,Yazılımcı</t>
-  </si>
-  <si>
-    <t>Bireysel</t>
+    <t>T50</t>
+  </si>
+  <si>
+    <t>Araştırmacı,Yazılımcı</t>
+  </si>
+  <si>
+    <t>T54</t>
+  </si>
+  <si>
+    <t>Yardımcı</t>
   </si>
 </sst>
 </file>
@@ -591,27 +600,27 @@
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="1">
-        <v>49</v>
+      <c r="A2" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="1">
-        <v>50</v>
+      <c r="A3" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="1">
-        <v>55</v>
+      <c r="A4" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>